<commit_message>
menambahkan informasi terkait software yang harus diinstall ke laptop peserta pribadi
</commit_message>
<xml_diff>
--- a/Template Data Email Konfirmasi.xlsx
+++ b/Template Data Email Konfirmasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wahyu/Documents/kumpulan file coding/coding_kerjaan/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9278DB-98D7-0740-90EC-8A587CD85070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B7BBF8-A27B-0E41-AF0E-65D30AC38B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="9000" windowWidth="30240" windowHeight="18880" xr2:uid="{617A867B-F7AD-014C-94B7-7383ABA0291C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{617A867B-F7AD-014C-94B7-7383ABA0291C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t xml:space="preserve">NAMA TRAINING: </t>
   </si>
@@ -121,9 +121,6 @@
     <t>Link Lokasi by Gmaps</t>
   </si>
   <si>
-    <t>xpkgvdxxanhkahow</t>
-  </si>
-  <si>
     <t>https://maps.app.goo.gl/Y1x6frkgPUzXRvrH8</t>
   </si>
   <si>
@@ -158,13 +155,40 @@
   </si>
   <si>
     <t>Inhouse Training Testing Brainmatics Training</t>
+  </si>
+  <si>
+    <t>------------</t>
+  </si>
+  <si>
+    <t>Enterprise Architecture</t>
+  </si>
+  <si>
+    <t>Link Download Software:</t>
+  </si>
+  <si>
+    <t>bit.ly/download-software</t>
+  </si>
+  <si>
+    <t>Jumlah Software:</t>
+  </si>
+  <si>
+    <t>Software Yang harus Diinstall</t>
+  </si>
+  <si>
+    <t>yusuf@brainmatics.com</t>
+  </si>
+  <si>
+    <t>GAJAHterbang123_</t>
+  </si>
+  <si>
+    <t>SOFTWARE YANG HARUS DIINSTALL OLEH PESERTA JIKA PESERTA MENGGUNAKAN LAPTOP PRIBADI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -202,6 +226,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -217,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -273,12 +305,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -304,7 +349,13 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -622,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575F8A91-AE8A-DE4C-9B89-20486B2D5914}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,8 +685,8 @@
     <col min="4" max="4" width="30" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
     <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="23" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -644,8 +695,12 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>40</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -666,6 +721,12 @@
       <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -681,10 +742,16 @@
         <v>19</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -695,18 +762,17 @@
         <v>16</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="1"/>
       <c r="I5" s="9"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -714,21 +780,23 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="13"/>
+      <c r="H6" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -738,13 +806,13 @@
         <v>17</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>20</v>
@@ -758,16 +826,19 @@
         <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>20</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -775,6 +846,9 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
+      <c r="H9" s="13" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -784,6 +858,7 @@
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="5"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -791,6 +866,7 @@
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="5"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -803,50 +879,55 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="5"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="5"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="5"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -854,92 +935,103 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="5"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="5"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1000,6 +1092,9 @@
       <c r="F41" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H2:I2"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{7419BAA3-2E79-4D40-BF69-2872E3F946DA}"/>
@@ -1007,7 +1102,7 @@
     <hyperlink ref="D6" r:id="rId3" xr:uid="{EC7953FA-D24C-6D45-8495-04ACCC5420B0}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{1D7AF929-E86B-E04E-8F1A-18A92A508B61}"/>
     <hyperlink ref="D8" r:id="rId5" xr:uid="{154A1716-5683-014A-B322-9DA882D985E6}"/>
-    <hyperlink ref="B13" r:id="rId6" display="mailto:maulanayuusuf023@gmail.com" xr:uid="{76D9C3A4-CEE1-4349-B1CE-D322793FAE3E}"/>
+    <hyperlink ref="B13" r:id="rId6" xr:uid="{76D9C3A4-CEE1-4349-B1CE-D322793FAE3E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add format body email for 1h online training
</commit_message>
<xml_diff>
--- a/Template Data Email Konfirmasi.xlsx
+++ b/Template Data Email Konfirmasi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wahyu/Documents/kumpulan file coding/coding_kerjaan/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47590E49-CE17-F548-97D5-ADFFD9642BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F4FDE8-1CF0-BB47-9772-75C18682043F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{617A867B-F7AD-014C-94B7-7383ABA0291C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{617A867B-F7AD-014C-94B7-7383ABA0291C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve">NAMA TRAINING: </t>
   </si>
@@ -160,15 +160,9 @@
     <t>------------</t>
   </si>
   <si>
-    <t>Enterprise Architecture</t>
-  </si>
-  <si>
     <t>Link Download Software:</t>
   </si>
   <si>
-    <t>bit.ly/download-software</t>
-  </si>
-  <si>
     <t>Jumlah Software:</t>
   </si>
   <si>
@@ -182,13 +176,37 @@
   </si>
   <si>
     <t>SOFTWARE YANG HARUS DIINSTALL OLEH PESERTA JIKA PESERTA MENGGUNAKAN LAPTOP PRIBADI</t>
+  </si>
+  <si>
+    <t>DIISI Jika Online Training atau Via ZOOM</t>
+  </si>
+  <si>
+    <t>Meeting ID:</t>
+  </si>
+  <si>
+    <t>Password Zoom Meeting:</t>
+  </si>
+  <si>
+    <t>Link Join Online Training:</t>
+  </si>
+  <si>
+    <t>contoh</t>
+  </si>
+  <si>
+    <t>Hari Online Training:</t>
+  </si>
+  <si>
+    <t>zoom.com</t>
+  </si>
+  <si>
+    <t>Minggu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -234,8 +252,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,6 +271,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -355,6 +387,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -673,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575F8A91-AE8A-DE4C-9B89-20486B2D5914}">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,7 +736,7 @@
         <v>39</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I2" s="15"/>
     </row>
@@ -722,10 +760,10 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -748,10 +786,7 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -838,7 +873,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -846,9 +881,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="5"/>
-      <c r="H9" s="13" t="s">
-        <v>41</v>
-      </c>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -886,7 +919,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -919,7 +952,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -945,9 +978,7 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>5</v>
-      </c>
+      <c r="A19" s="4"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -962,6 +993,10 @@
       <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="17"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -969,6 +1004,8 @@
       <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -983,6 +1020,9 @@
       <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -990,18 +1030,36 @@
       <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
@@ -1092,8 +1150,9 @@
       <c r="F41" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="H2:I2"/>
+    <mergeCell ref="A21:B22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
add regular/private online training format - request by restu
</commit_message>
<xml_diff>
--- a/Template Data Email Konfirmasi.xlsx
+++ b/Template Data Email Konfirmasi.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wahyu/Documents/kumpulan file coding/coding_kerjaan/python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F4FDE8-1CF0-BB47-9772-75C18682043F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29CD39F-A2EF-4F4C-AA88-666A0573C3BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{617A867B-F7AD-014C-94B7-7383ABA0291C}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{617A867B-F7AD-014C-94B7-7383ABA0291C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="63">
   <si>
     <t xml:space="preserve">NAMA TRAINING: </t>
   </si>
@@ -154,9 +154,6 @@
     <t>831-4937-2243</t>
   </si>
   <si>
-    <t>Inhouse Training Testing Brainmatics Training</t>
-  </si>
-  <si>
     <t>------------</t>
   </si>
   <si>
@@ -200,6 +197,33 @@
   </si>
   <si>
     <t>Minggu</t>
+  </si>
+  <si>
+    <t>Tipe Online Training:</t>
+  </si>
+  <si>
+    <t>ROT</t>
+  </si>
+  <si>
+    <t>(Pilih Salah Satu, ROT, POT atau 1H)</t>
+  </si>
+  <si>
+    <t>ROT =&gt; Regular Online Training</t>
+  </si>
+  <si>
+    <t>POT =&gt; Private Online Training</t>
+  </si>
+  <si>
+    <t>1H =&gt; 1Hour Online Training</t>
+  </si>
+  <si>
+    <t>===</t>
+  </si>
+  <si>
+    <t>11222 3344</t>
+  </si>
+  <si>
+    <t>Private Online Training Testing Brainmatics Training</t>
   </si>
 </sst>
 </file>
@@ -709,10 +733,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{575F8A91-AE8A-DE4C-9B89-20486B2D5914}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,10 +758,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I2" s="15"/>
     </row>
@@ -760,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -786,7 +811,7 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -830,7 +855,7 @@
         <v>20</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -873,7 +898,7 @@
         <v>20</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -919,7 +944,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -952,7 +977,7 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -994,7 +1019,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B21" s="17"/>
       <c r="C21" s="6"/>
@@ -1021,7 +1046,10 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>48</v>
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
@@ -1031,10 +1059,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -1043,10 +1071,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
@@ -1055,10 +1083,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -1078,72 +1106,94 @@
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>55</v>
+      </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="1"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>57</v>
+      </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
       <c r="E33" s="6"/>
       <c r="F33" s="5"/>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>58</v>
+      </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="5"/>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="5"/>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="5"/>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>

</xml_diff>